<commit_message>
Add AliOcrClientActivity and use it in bank card unit test.
</commit_message>
<xml_diff>
--- a/tests/AliOcrBasicTests/Tests_Data/config/ali_ocr_config.xlsx
+++ b/tests/AliOcrBasicTests/Tests_Data/config/ali_ocr_config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allenlooplee\Documents\GitHub\AliOcrActivitiesPack\tests\AliOcrBasicTests\Tests_Data\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0F785E-9B0B-40F7-954C-FD0609016B84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C51CF6CA-6747-476A-9992-307CABBBB735}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2580" yWindow="1845" windowWidth="16200" windowHeight="9397" xr2:uid="{D6D768DA-5964-4C9E-A98A-0598DDF1AEA9}"/>
   </bookViews>
@@ -461,7 +461,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>